<commit_message>
mais um update, a partir de agora é sempre a abrir
</commit_message>
<xml_diff>
--- a/Lista de Tarefas.xlsx
+++ b/Lista de Tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Lista de Tarefas a Realizar</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Meter prints dos acontecimentos no servidor</t>
   </si>
   <si>
-    <t>Data de realização</t>
-  </si>
-  <si>
     <t>Corrigir layouts</t>
   </si>
   <si>
@@ -82,6 +79,21 @@
   </si>
   <si>
     <t>Feedback de operações na aplicação movel</t>
+  </si>
+  <si>
+    <t>Problemas de Toasts</t>
+  </si>
+  <si>
+    <t>Mudar Class do MyApplication para usar os helpers</t>
+  </si>
+  <si>
+    <t>Completar Helpers</t>
+  </si>
+  <si>
+    <t>% de Completude</t>
+  </si>
+  <si>
+    <t>Spinner Cozinha</t>
   </si>
 </sst>
 </file>
@@ -125,11 +137,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,17 +451,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D24"/>
+  <dimension ref="B3:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="80.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -451,156 +469,252 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
         <v>3</v>
       </c>
       <c r="D5" s="3">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
       </c>
       <c r="D7" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
       </c>
       <c r="D8" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
       </c>
       <c r="D11" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
       </c>
       <c r="D12" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5</v>
       </c>
       <c r="D13" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="3">
-        <v>2</v>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C23" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alteraçoes principalmente na class main
</commit_message>
<xml_diff>
--- a/Lista de Tarefas.xlsx
+++ b/Lista de Tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Lista de Tarefas a Realizar</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Spinner Cozinha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O que está a precisar de ser mesmo tratado é o modo automático. Fazer com que o dia/noite e </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> app aquilo esteja a funcionar correctamente. Os pontos da sala 124 tambem sao importantes.</t>
+  </si>
+  <si>
+    <t>O dia/noite e bom/mau tempo nao ta a ser enviado para a app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bom/mau tempo afectem as janelas/luz e depois quando mexermos nas janelas e luzes na </t>
   </si>
 </sst>
 </file>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:D28"/>
+  <dimension ref="B3:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,6 +725,26 @@
     <row r="28" spans="2:4">
       <c r="B28" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>